<commit_message>
Updated address override APIs
</commit_message>
<xml_diff>
--- a/TF_UI_APIs.xlsx
+++ b/TF_UI_APIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\W\tf-new-arch-artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF256E5-A322-49D2-8C3C-F26507A10843}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5A0CA7-1EEB-445B-88AC-56EBD2FCB6C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="234">
   <si>
     <t>Tax Authority</t>
   </si>
@@ -759,6 +759,12 @@
   </si>
   <si>
     <t>/TaxCodeService/deleteAddressOverride</t>
+  </si>
+  <si>
+    <t>PlaceCode,SchoolDistrict,Counties,AddOvrdState</t>
+  </si>
+  <si>
+    <t>/TaxCodeService/deleteRedundantAddressOverrides</t>
   </si>
 </sst>
 </file>
@@ -2519,17 +2525,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.140625" customWidth="1"/>
     <col min="4" max="4" width="47.7109375" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="42" customWidth="1"/>
@@ -2602,6 +2608,9 @@
       <c r="B2" t="s">
         <v>63</v>
       </c>
+      <c r="C2" t="s">
+        <v>232</v>
+      </c>
       <c r="D2" t="s">
         <v>227</v>
       </c>
@@ -2630,6 +2639,12 @@
         <v>230</v>
       </c>
       <c r="M2" t="s">
+        <v>66</v>
+      </c>
+      <c r="N2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O2" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3102,6 +3117,11 @@
       </c>
       <c r="M12" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated unemployment override APIs
</commit_message>
<xml_diff>
--- a/TF_UI_APIs.xlsx
+++ b/TF_UI_APIs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\W\tf-new-arch-artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5A0CA7-1EEB-445B-88AC-56EBD2FCB6C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE412749-E531-4071-8F3D-ABE9497BAD80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Type1" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="241">
   <si>
     <t>Tax Authority</t>
   </si>
@@ -765,6 +765,27 @@
   </si>
   <si>
     <t>/TaxCodeService/deleteRedundantAddressOverrides</t>
+  </si>
+  <si>
+    <t>unemploymentOverrides</t>
+  </si>
+  <si>
+    <t>AuthorityCodeList,TaxTypes,FormulaUnemp</t>
+  </si>
+  <si>
+    <t>/TaxCodeService/getUnempOverrideList</t>
+  </si>
+  <si>
+    <t>/TaxCodeService/saveUnemploymentOverride</t>
+  </si>
+  <si>
+    <t>/TaxCodeService/deleteUnemploymentOverride</t>
+  </si>
+  <si>
+    <t>Extra APIs</t>
+  </si>
+  <si>
+    <t>Extra APIs Ready</t>
   </si>
 </sst>
 </file>
@@ -2190,8 +2211,8 @@
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="Get URL Ready?"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Edit Entity"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0300-000010000000}" name="Edit  URL Ready"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0300-000011000000}" name="Get Usage URL"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0300-000012000000}" name="Get Usage Ready"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0300-000011000000}" name="Extra APIs"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0300-000012000000}" name="Extra APIs Ready"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Delete URL"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0300-00000D000000}" name="Delete Ready?"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Save/Update URL"/>
@@ -2527,8 +2548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4458,15 +4479,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
     <col min="4" max="4" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.5703125" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
@@ -4474,9 +4495,9 @@
     <col min="8" max="8" width="16.5703125" customWidth="1"/>
     <col min="9" max="9" width="36.28515625" customWidth="1"/>
     <col min="10" max="10" width="16.5703125" customWidth="1"/>
-    <col min="11" max="11" width="40.5703125" customWidth="1"/>
+    <col min="11" max="11" width="46.7109375" customWidth="1"/>
     <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="38.85546875" customWidth="1"/>
+    <col min="13" max="13" width="45.140625" customWidth="1"/>
     <col min="14" max="14" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
@@ -4509,10 +4530,10 @@
         <v>144</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>145</v>
+        <v>239</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>146</v>
+        <v>240</v>
       </c>
       <c r="K1" s="10" t="s">
         <v>68</v>
@@ -4627,6 +4648,45 @@
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>187</v>
+      </c>
+      <c r="B4" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" t="s">
+        <v>236</v>
+      </c>
+      <c r="F4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K4" t="s">
+        <v>238</v>
+      </c>
+      <c r="L4" t="s">
+        <v>66</v>
+      </c>
+      <c r="M4" t="s">
+        <v>237</v>
+      </c>
+      <c r="N4" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pension What If API
</commit_message>
<xml_diff>
--- a/TF_UI_APIs.xlsx
+++ b/TF_UI_APIs.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\W\tf-new-arch-artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CFEA61-09C0-467E-BECD-9F27126B8B23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB52185-0403-45A8-A875-7A58AE590C26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3990" yWindow="45" windowWidth="21705" windowHeight="14835" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Type1" sheetId="2" r:id="rId1"/>
     <sheet name="UDQ Filters" sheetId="3" r:id="rId2"/>
     <sheet name="UDQ" sheetId="1" r:id="rId3"/>
     <sheet name="Type 2" sheetId="4" r:id="rId4"/>
-    <sheet name="API Spec-Test" sheetId="5" r:id="rId5"/>
-    <sheet name="Reporting Too" sheetId="6" r:id="rId6"/>
+    <sheet name="Pension What if" sheetId="7" r:id="rId5"/>
+    <sheet name="API Spec-Test" sheetId="5" r:id="rId6"/>
+    <sheet name="Reporting Too" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="285">
   <si>
     <t>Tax Authority</t>
   </si>
@@ -892,6 +893,33 @@
   </si>
   <si>
     <t>deleteAllMessagesByRunId</t>
+  </si>
+  <si>
+    <t>/WhatIfService/getPensionWhatIfEmployees</t>
+  </si>
+  <si>
+    <t>/WhatIfService/deleteAllPensionWhatIfEmployees</t>
+  </si>
+  <si>
+    <t>/WhatIfService/savePensionRecipient</t>
+  </si>
+  <si>
+    <t>/WhatIfService/updatePensionRecipient</t>
+  </si>
+  <si>
+    <t>/WhatIfService/deletePensionRecipient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/WhatIfService/saveAsPensionRecipient </t>
+  </si>
+  <si>
+    <t>/WhatIfService/generatePensionRecipientPDF</t>
+  </si>
+  <si>
+    <t>Pension What If Taxes</t>
+  </si>
+  <si>
+    <t>Pension What If Recipient</t>
   </si>
 </sst>
 </file>
@@ -1110,7 +1138,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1190,6 +1218,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2925,7 +2956,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3536,7 +3567,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5219,6 +5250,69 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C1C95F1-B491-4EFF-B631-D7340BA4B41F}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="62.140625" customWidth="1"/>
+    <col min="2" max="2" width="57.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>282</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:H410"/>
   <sheetViews>
@@ -10161,11 +10255,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Optional Rate Overrides API
</commit_message>
<xml_diff>
--- a/TF_UI_APIs.xlsx
+++ b/TF_UI_APIs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\W\tf-new-arch-artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58D8ED9-BC51-453E-AD60-6275AA287645}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70095FE7-5F8F-4AE9-939D-78BB62C325C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Type1" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="402">
   <si>
     <t>Tax Authority</t>
   </si>
@@ -1257,6 +1257,24 @@
   </si>
   <si>
     <t>/TaxCodeService/getRecipOvrdAutocompleteNonResTaxTypesLocal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">public ResponseEntity&lt;List&lt;OptionalRateOverride&gt;&gt; getOptionalRateOverrides(@Valid @NotNull @RequestBody(required = true) InputData input) throws Exception </t>
+  </si>
+  <si>
+    <t>public ResponseEntity&lt;FormOutput&gt; saveOptionalRateOverride(@Valid @NotNull @RequestBody(required = true) OptionalRateOverride optionalRateOverride) throws Exception</t>
+  </si>
+  <si>
+    <t>public ResponseEntity&lt;FormOutput&gt; deleteOptionalRateOverride(@Valid @NotNull @RequestBody(required = true) OptionalRateOverride optionalRateOverride) throws Exception</t>
+  </si>
+  <si>
+    <t>public ResponseEntity&lt;List&lt;Object&gt;&gt; getAuthoritiesAutocomplete(@Valid @NotNull @RequestBody(required = true) InputData input) throws Exception</t>
+  </si>
+  <si>
+    <t>public ResponseEntity&lt;List&lt;Object&gt;&gt; getTaxTypesAutocomplete(@Valid @NotNull @RequestBody(required = true) InputData input) throws Exception</t>
+  </si>
+  <si>
+    <t>public ResponseEntity&lt;List&lt;Object&gt;&gt; getFormulaAutocomplete(@Valid @NotNull @RequestBody(required = true) InputData input) throws Exception</t>
   </si>
 </sst>
 </file>
@@ -11150,10 +11168,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11201,6 +11219,41 @@
         <v>377</v>
       </c>
     </row>
+    <row r="10" spans="1:1" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="47" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>401</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -11211,7 +11264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Custom Garnishment Formulas API
</commit_message>
<xml_diff>
--- a/TF_UI_APIs.xlsx
+++ b/TF_UI_APIs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\W\tf-new-arch-artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8FEE12-31EA-4BC7-B25A-9939AB75E3FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD992C5-14AE-4261-A925-039AAF431802}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Type1" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="417">
   <si>
     <t>Tax Authority</t>
   </si>
@@ -1277,9 +1277,6 @@
     <t>public ResponseEntity&lt;List&lt;Object&gt;&gt; getFormulaAutocomplete(@Valid @NotNull @RequestBody(required = true) InputData input) throws Exception</t>
   </si>
   <si>
-    <t>calculateBsiWage</t>
-  </si>
-  <si>
     <t>/CompanyService/getOptionalRateOverrides</t>
   </si>
   <si>
@@ -1302,6 +1299,27 @@
   </si>
   <si>
     <t>/CompanyService/calculateBsiWage</t>
+  </si>
+  <si>
+    <t>/TaxCodeService/getCustomGarnishmentFormulas</t>
+  </si>
+  <si>
+    <t>/TaxCodeService/getCustomGarnishmentFormulaDetail</t>
+  </si>
+  <si>
+    <t>/TaxCodeService/deleteCustomGarnishmentFormula</t>
+  </si>
+  <si>
+    <t>/TaxCodeService/saveCustomGarnishmentFormula</t>
+  </si>
+  <si>
+    <t>/TaxCodeService/updateCustomGarnishmentFormula</t>
+  </si>
+  <si>
+    <t>/TaxCodeService/generateCustomGarnishmentFormulaPDF</t>
+  </si>
+  <si>
+    <t>/TaxCodeService/autocompleteCustomGarnishments</t>
   </si>
 </sst>
 </file>
@@ -3338,7 +3356,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11289,10 +11307,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11301,10 +11319,11 @@
     <col min="2" max="2" width="41" customWidth="1"/>
     <col min="3" max="3" width="61.42578125" customWidth="1"/>
     <col min="4" max="4" width="64.42578125" customWidth="1"/>
-    <col min="5" max="5" width="56.28515625" customWidth="1"/>
+    <col min="5" max="5" width="58.5703125" customWidth="1"/>
+    <col min="6" max="6" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="47" t="s">
         <v>215</v>
       </c>
@@ -11320,8 +11339,11 @@
       <c r="E1" s="47" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="47" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>175</v>
       </c>
@@ -11337,8 +11359,11 @@
       <c r="E2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>364</v>
       </c>
@@ -11352,10 +11377,13 @@
         <v>248</v>
       </c>
       <c r="E3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+      <c r="F3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>365</v>
       </c>
@@ -11366,10 +11394,13 @@
         <v>251</v>
       </c>
       <c r="E4" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+      <c r="F4" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>366</v>
       </c>
@@ -11380,10 +11411,13 @@
         <v>387</v>
       </c>
       <c r="E5" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>404</v>
+      </c>
+      <c r="F5" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>360</v>
       </c>
@@ -11394,10 +11428,13 @@
         <v>388</v>
       </c>
       <c r="E6" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>405</v>
+      </c>
+      <c r="F6" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>367</v>
       </c>
@@ -11408,10 +11445,13 @@
         <v>389</v>
       </c>
       <c r="E7" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>406</v>
+      </c>
+      <c r="F7" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>368</v>
       </c>
@@ -11422,10 +11462,13 @@
         <v>390</v>
       </c>
       <c r="E8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+      <c r="F8" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>369</v>
       </c>
@@ -11436,10 +11479,13 @@
         <v>391</v>
       </c>
       <c r="E9" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>408</v>
+      </c>
+      <c r="F9" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>370</v>
       </c>
@@ -11447,20 +11493,20 @@
         <v>392</v>
       </c>
       <c r="E10" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>395</v>
       </c>

</xml_diff>

<commit_message>
Custom Nexus Data API
</commit_message>
<xml_diff>
--- a/TF_UI_APIs.xlsx
+++ b/TF_UI_APIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\W\tf-new-arch-artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD992C5-14AE-4261-A925-039AAF431802}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8515E1-67C0-4262-A2F1-FC53ED44EF56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="421">
   <si>
     <t>Tax Authority</t>
   </si>
@@ -1320,6 +1320,18 @@
   </si>
   <si>
     <t>/TaxCodeService/autocompleteCustomGarnishments</t>
+  </si>
+  <si>
+    <t>/CompanyService/getCustomNexusList</t>
+  </si>
+  <si>
+    <t>/CompanyService/deleteCustomNexusData</t>
+  </si>
+  <si>
+    <t>/CompanyService/saveCustomNexusData</t>
+  </si>
+  <si>
+    <t>/CompanyService/autocompleteCustNexusAuthorities</t>
   </si>
 </sst>
 </file>
@@ -11307,10 +11319,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11511,6 +11523,36 @@
         <v>395</v>
       </c>
     </row>
+    <row r="17" spans="1:1" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="47" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>420</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Custom Payment Exceptions API
</commit_message>
<xml_diff>
--- a/TF_UI_APIs.xlsx
+++ b/TF_UI_APIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\W\tf-new-arch-artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8515E1-67C0-4262-A2F1-FC53ED44EF56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AF838C-FAAB-42D8-8025-ADF5234DECA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="426">
   <si>
     <t>Tax Authority</t>
   </si>
@@ -1332,6 +1332,21 @@
   </si>
   <si>
     <t>/CompanyService/autocompleteCustNexusAuthorities</t>
+  </si>
+  <si>
+    <t>/PaymentsService/getCustomPaymentsForExceptions</t>
+  </si>
+  <si>
+    <t>/PaymentsService/getCustomPaymentExceptions</t>
+  </si>
+  <si>
+    <t>/PaymentsService/getCustomPaymentExceptionDetail</t>
+  </si>
+  <si>
+    <t>/PaymentsService/deleteCustomPaymentException</t>
+  </si>
+  <si>
+    <t>/PaymentsService/saveCustomPaymentException</t>
   </si>
 </sst>
 </file>
@@ -3368,7 +3383,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11319,16 +11334,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66.85546875" customWidth="1"/>
-    <col min="2" max="2" width="41" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" customWidth="1"/>
     <col min="3" max="3" width="61.42578125" customWidth="1"/>
     <col min="4" max="4" width="64.42578125" customWidth="1"/>
     <col min="5" max="5" width="58.5703125" customWidth="1"/>
@@ -11523,34 +11538,62 @@
         <v>395</v>
       </c>
     </row>
-    <row r="17" spans="1:1" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="47" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" s="47" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>420</v>
+      </c>
+      <c r="B22" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Custom Tax Payment Overrides API
</commit_message>
<xml_diff>
--- a/TF_UI_APIs.xlsx
+++ b/TF_UI_APIs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\W\tf-new-arch-artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AF838C-FAAB-42D8-8025-ADF5234DECA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A9A03C-4883-46A8-A8F0-187B39FA0198}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Type1" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="430">
   <si>
     <t>Tax Authority</t>
   </si>
@@ -1347,6 +1347,18 @@
   </si>
   <si>
     <t>/PaymentsService/saveCustomPaymentException</t>
+  </si>
+  <si>
+    <t>/TaxCodeService/getCustomTaxPaymentOverrides</t>
+  </si>
+  <si>
+    <t>/TaxCodeService/saveCustomTaxPaymentOverride</t>
+  </si>
+  <si>
+    <t>/TaxCodeService/deleteCustomTaxPaymentOverride</t>
+  </si>
+  <si>
+    <t>/UserDataQueriesService/getAutocomplete...ToolsSelectFieldIds.TaxTypesPymtOvrd</t>
   </si>
 </sst>
 </file>
@@ -1565,7 +1577,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1648,6 +1660,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3383,7 +3398,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9130,7 +9145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -9681,7 +9696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -10830,7 +10845,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10934,7 +10949,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11337,7 +11352,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11538,60 +11553,81 @@
         <v>395</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="47" t="s">
         <v>193</v>
       </c>
       <c r="B17" s="47" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="47" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>111</v>
       </c>
       <c r="B18" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>417</v>
       </c>
       <c r="B19" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>418</v>
       </c>
       <c r="B20" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>419</v>
       </c>
       <c r="B21" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>420</v>
       </c>
       <c r="B22" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="48" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>86</v>
       </c>

</xml_diff>

<commit_message>
Connect To Dataset API
</commit_message>
<xml_diff>
--- a/TF_UI_APIs.xlsx
+++ b/TF_UI_APIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\W\tf-new-arch-artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8CD120-9F05-4659-ACC0-580E3B669685}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DC24F4-06ED-4139-B8A9-EF3B06585CD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="506">
   <si>
     <t>Tax Authority</t>
   </si>
@@ -1572,6 +1572,21 @@
   </si>
   <si>
     <t>/MappingToolsService/getPaymentCodeUsage</t>
+  </si>
+  <si>
+    <t>Connect To Dataset</t>
+  </si>
+  <si>
+    <t>/DatasetService/getDatasetsForLogin</t>
+  </si>
+  <si>
+    <t>/DatasetService/isManageLogins</t>
+  </si>
+  <si>
+    <t>/DatasetService/isManageDatasets</t>
+  </si>
+  <si>
+    <t>/DatasetService/connectDataset</t>
   </si>
 </sst>
 </file>
@@ -11562,10 +11577,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12102,14 +12117,39 @@
         <v>470</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>472</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="47" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>505</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Custom BackUp Restore Datasets API
</commit_message>
<xml_diff>
--- a/TF_UI_APIs.xlsx
+++ b/TF_UI_APIs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\W\tf-new-arch-artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312CA548-7B1E-4A13-A184-C4BEA3C0A6AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739C405B-A1BA-47FA-B205-6B8C33A7DD8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="519">
   <si>
     <t>Tax Authority</t>
   </si>
@@ -1605,6 +1605,27 @@
   </si>
   <si>
     <t>/DatasetService/deleteAllAudit</t>
+  </si>
+  <si>
+    <t>Custom BackUp Restore Datasets</t>
+  </si>
+  <si>
+    <t>/FileUploaderService/getCustomBackupRestoreInfo</t>
+  </si>
+  <si>
+    <t>/FileUploaderService/backupDatasets</t>
+  </si>
+  <si>
+    <t>/FileUploaderService/uploadRestoreDatasetFile</t>
+  </si>
+  <si>
+    <t>/FileUploaderService/restoreDatasets</t>
+  </si>
+  <si>
+    <t>/FileUploaderService/getBackUpRestoreStatus</t>
+  </si>
+  <si>
+    <t>/FileUploaderService/backupRestoreOutputFiles</t>
   </si>
 </sst>
 </file>
@@ -11595,10 +11616,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54:B58"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54:C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12135,59 +12156,87 @@
         <v>470</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="53" spans="1:2" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="47" t="s">
         <v>501</v>
       </c>
       <c r="B53" s="47" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53" s="47" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>502</v>
       </c>
       <c r="B54" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>503</v>
       </c>
       <c r="B55" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>504</v>
       </c>
       <c r="B56" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>505</v>
       </c>
       <c r="B57" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>511</v>
+      </c>
+      <c r="C58" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Custom BackUp Restore Rate API
</commit_message>
<xml_diff>
--- a/TF_UI_APIs.xlsx
+++ b/TF_UI_APIs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\W\tf-new-arch-artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739C405B-A1BA-47FA-B205-6B8C33A7DD8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6974E38-8DFA-4CA4-ABBC-7604C1210253}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="522">
   <si>
     <t>Tax Authority</t>
   </si>
@@ -1626,6 +1626,15 @@
   </si>
   <si>
     <t>/FileUploaderService/backupRestoreOutputFiles</t>
+  </si>
+  <si>
+    <t>Custom BackUp Restore Rate Overrides</t>
+  </si>
+  <si>
+    <t>/FileUploaderService/backupRateOverrides</t>
+  </si>
+  <si>
+    <t>/FileUploaderService/restoreRateOverrides</t>
   </si>
 </sst>
 </file>
@@ -11618,8 +11627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54:C60"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12156,17 +12165,17 @@
         <v>470</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="47" t="s">
         <v>501</v>
       </c>
@@ -12176,8 +12185,11 @@
       <c r="C53" s="47" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" s="47" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>502</v>
       </c>
@@ -12185,10 +12197,13 @@
         <v>507</v>
       </c>
       <c r="C54" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+      <c r="D54" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>503</v>
       </c>
@@ -12198,8 +12213,11 @@
       <c r="C55" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>504</v>
       </c>
@@ -12209,8 +12227,11 @@
       <c r="C56" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>505</v>
       </c>
@@ -12220,8 +12241,11 @@
       <c r="C57" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>511</v>
       </c>
@@ -12229,12 +12253,12 @@
         <v>516</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>518</v>
       </c>

</xml_diff>

<commit_message>
adding postman test cases
</commit_message>
<xml_diff>
--- a/TF_UI_APIs.xlsx
+++ b/TF_UI_APIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\W\tf-new-arch-artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21CB9CF-BDF7-4C48-BC19-3FB2B8F4E18D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9E76EE-D7C0-4E2D-9DDF-7FF591D3FB49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="534">
   <si>
     <t>Tax Authority</t>
   </si>
@@ -1650,6 +1650,27 @@
   </si>
   <si>
     <t>/FileUploaderService/databaseLoadOutputFiles</t>
+  </si>
+  <si>
+    <t>Machine Key</t>
+  </si>
+  <si>
+    <t>/FileUploaderService/installMachineKey</t>
+  </si>
+  <si>
+    <t>Manual Update</t>
+  </si>
+  <si>
+    <t>/FileUploaderService/generateBulletinListPDF</t>
+  </si>
+  <si>
+    <t>/FileUploaderService/getManualUploadStatus</t>
+  </si>
+  <si>
+    <t>/FileUploaderService/manualUpdate</t>
+  </si>
+  <si>
+    <t>/FileUploaderService/manualUpdateOutputFiles</t>
   </si>
 </sst>
 </file>
@@ -11640,10 +11661,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63:B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12293,6 +12314,37 @@
         <v>518</v>
       </c>
     </row>
+    <row r="62" spans="1:5" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="47" t="s">
+        <v>527</v>
+      </c>
+      <c r="B62" s="47" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>528</v>
+      </c>
+      <c r="B63" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>533</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Messages to Suppress APIs
</commit_message>
<xml_diff>
--- a/TF_UI_APIs.xlsx
+++ b/TF_UI_APIs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\W\tf-new-arch-artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD53B0B-5E46-41A6-BD89-FD6566F584FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F376706-FE43-43B6-9D35-CCE2EAE64598}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="545">
   <si>
     <t>Tax Authority</t>
   </si>
@@ -1692,6 +1692,18 @@
   </si>
   <si>
     <t>/DatasetService/getAboutPageInfo</t>
+  </si>
+  <si>
+    <t>Messages To Suppress</t>
+  </si>
+  <si>
+    <t>/MessageService/getMessagesToSuppress</t>
+  </si>
+  <si>
+    <t>/MessageService/resetMessagesToSuppress</t>
+  </si>
+  <si>
+    <t>/MessageService/saveMessagesToSuppress</t>
   </si>
 </sst>
 </file>
@@ -11684,8 +11696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63:D64"/>
+    <sheetView tabSelected="1" topLeftCell="C45" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63:E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12348,6 +12360,9 @@
       <c r="D62" s="47" t="s">
         <v>538</v>
       </c>
+      <c r="E62" s="47" t="s">
+        <v>541</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
@@ -12362,6 +12377,9 @@
       <c r="D63" t="s">
         <v>539</v>
       </c>
+      <c r="E63" t="s">
+        <v>542</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
@@ -12373,16 +12391,22 @@
       <c r="D64" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>532</v>
       </c>
       <c r="C65" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>533</v>
       </c>

</xml_diff>